<commit_message>
Formule seuil rentabilité linéaire
</commit_message>
<xml_diff>
--- a/01. Recherche opérationnelle (Operations research - Management science)/01. Linéaire/00 - SEUIL DE RENTABILITE(EVEN BREAKPOINT)/Formule du seuil de rentabilité.xlsx
+++ b/01. Recherche opérationnelle (Operations research - Management science)/01. Linéaire/00 - SEUIL DE RENTABILITE(EVEN BREAKPOINT)/Formule du seuil de rentabilité.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="360" yWindow="120" windowWidth="11280" windowHeight="6228"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Calcul seuil rentabilité" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
@@ -239,6 +239,169 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>175846</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>82061</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>556846</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>93785</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4443046" y="252046"/>
+          <a:ext cx="3429000" cy="2901462"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" b="1"/>
+            <a:t>Formule de calcul des couts : </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR"/>
+            <a:t>total cost = total fixed cost + total variable cost</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>cout variables = cout par jean</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>cout fixe = cout total de l'usine</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Formule de calcul du profit : </a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR"/>
+            <a:t>total profit = total revenue - total cost</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR"/>
+            <a:t>Z = vp - cf - vcv</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" b="1"/>
+            <a:t>Formule</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" b="1" baseline="0"/>
+            <a:t> du seuil de rentabilité : </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR"/>
+            <a:t>v = couts fixes / prix - cout variable</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -531,7 +694,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -609,6 +772,7 @@
     <oddHeader>&amp;A</oddHeader>
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Seuil de rentabilité linéaire : formules
</commit_message>
<xml_diff>
--- a/01. Recherche opérationnelle (Operations research - Management science)/01. Linéaire/00 - SEUIL DE RENTABILITE(EVEN BREAKPOINT)/Formule du seuil de rentabilité.xlsx
+++ b/01. Recherche opérationnelle (Operations research - Management science)/01. Linéaire/00 - SEUIL DE RENTABILITE(EVEN BREAKPOINT)/Formule du seuil de rentabilité.xlsx
@@ -246,15 +246,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>175846</xdr:colOff>
+      <xdr:colOff>52754</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>82061</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>556846</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>93785</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -263,8 +263,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4443046" y="252046"/>
-          <a:ext cx="3429000" cy="2901462"/>
+          <a:off x="4319954" y="252046"/>
+          <a:ext cx="3552092" cy="4085492"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -325,23 +325,7 @@
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
         <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" b="1">
               <a:solidFill>
@@ -354,20 +338,128 @@
             </a:rPr>
             <a:t>Formule de calcul du profit : </a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR"/>
+          <a:endParaRPr lang="fr-FR">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>total profit = total revenue - total cost</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR"/>
+          <a:endParaRPr lang="fr-FR">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Z = vp - cf - vcv</a:t>
           </a:r>
+          <a:endParaRPr lang="fr-FR">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>oû</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>v =  volume de vente (i.e., demand) </a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>p = prix fixe</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>cf = cout</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>cv = cout variable</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="fr-FR"/>
@@ -386,6 +478,24 @@
           <a:r>
             <a:rPr lang="fr-FR"/>
             <a:t>v = couts fixes / prix - cout variable</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR"/>
+            <a:t>Source :</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR"/>
+            <a:t>Bernard_W_._Taylor_Introduction_to_Management_Science_11th_2013</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -693,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>